<commit_message>
update path, using os.path.join
</commit_message>
<xml_diff>
--- a/app/resource/xlsx/fee_proposal_template_2.xlsx
+++ b/app/resource/xlsx/fee_proposal_template_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeezh\xero-asana-intergration\app\resource\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zero\Documents\GitHub\xero-asana-intergration\app\resource\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BE0F45-019B-400A-BE6A-3F7938AB60BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8653EFAD-796E-40E5-A3AC-AC8DDA492B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F1EA209-DB64-4862-B5BC-AB2E13480384}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9F1EA209-DB64-4862-B5BC-AB2E13480384}"/>
   </bookViews>
   <sheets>
     <sheet name="Fee Proposal" sheetId="11" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="ClientCompany">#REF!</definedName>
     <definedName name="MainContactAddress">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Fee Proposal'!$A$1:$I$257</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Fee Proposal'!$A$1:$I$263</definedName>
     <definedName name="ProjectName">#REF!</definedName>
     <definedName name="ProjectType">#REF!</definedName>
     <definedName name="QuotationNumber">#REF!</definedName>
@@ -818,27 +818,45 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -856,24 +874,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -924,7 +924,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>323023</xdr:colOff>
-      <xdr:row>202</xdr:row>
+      <xdr:row>208</xdr:row>
       <xdr:rowOff>16567</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="737151" cy="746051"/>
@@ -969,13 +969,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>136</xdr:row>
+      <xdr:row>142</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>283770</xdr:colOff>
-      <xdr:row>138</xdr:row>
+      <xdr:row>144</xdr:row>
       <xdr:rowOff>58815</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1317,10 +1317,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96441BBC-02AB-4FA6-8E6A-4E6138E77562}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:X258"/>
+  <dimension ref="A1:X264"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A155" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="B178" sqref="B178:E178"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A107" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120:XFD120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1339,16 +1339,16 @@
       <c r="A1" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49" t="e">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47" t="e">
         <f>IF(#REF!&lt;&gt;"",#REF!,"")</f>
         <v>#REF!</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
     </row>
     <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="15"/>
@@ -1356,10 +1356,10 @@
       <c r="G2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
       <c r="O2" s="19"/>
@@ -1412,15 +1412,15 @@
       <c r="P5" s="14"/>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="63"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
       <c r="K6" s="18"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1472,14 +1472,14 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="60"/>
-      <c r="U9" s="60"/>
-      <c r="V9" s="60"/>
-      <c r="W9" s="60"/>
-      <c r="X9" s="60"/>
+      <c r="Q9" s="50"/>
+      <c r="R9" s="50"/>
+      <c r="S9" s="50"/>
+      <c r="T9" s="50"/>
+      <c r="U9" s="50"/>
+      <c r="V9" s="50"/>
+      <c r="W9" s="50"/>
+      <c r="X9" s="50"/>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1494,14 +1494,14 @@
       <c r="G11" s="48"/>
       <c r="H11" s="48"/>
       <c r="I11" s="48"/>
-      <c r="M11" s="61"/>
-      <c r="N11" s="61"/>
-      <c r="O11" s="61"/>
-      <c r="P11" s="61"/>
-      <c r="Q11" s="61"/>
-      <c r="R11" s="61"/>
-      <c r="S11" s="61"/>
-      <c r="T11" s="61"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="51"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="51"/>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="48"/>
@@ -1513,14 +1513,14 @@
       <c r="G12" s="48"/>
       <c r="H12" s="48"/>
       <c r="I12" s="48"/>
-      <c r="M12" s="61"/>
-      <c r="N12" s="61"/>
-      <c r="O12" s="61"/>
-      <c r="P12" s="61"/>
-      <c r="Q12" s="61"/>
-      <c r="R12" s="61"/>
-      <c r="S12" s="61"/>
-      <c r="T12" s="61"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="51"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="51"/>
     </row>
     <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="48"/>
@@ -1532,14 +1532,14 @@
       <c r="G13" s="48"/>
       <c r="H13" s="48"/>
       <c r="I13" s="48"/>
-      <c r="M13" s="61"/>
-      <c r="N13" s="61"/>
-      <c r="O13" s="61"/>
-      <c r="P13" s="61"/>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="61"/>
-      <c r="S13" s="61"/>
-      <c r="T13" s="61"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="51"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="51"/>
     </row>
     <row r="14" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48"/>
@@ -1551,14 +1551,14 @@
       <c r="G14" s="48"/>
       <c r="H14" s="48"/>
       <c r="I14" s="48"/>
-      <c r="M14" s="61"/>
-      <c r="N14" s="61"/>
-      <c r="O14" s="61"/>
-      <c r="P14" s="61"/>
-      <c r="Q14" s="61"/>
-      <c r="R14" s="61"/>
-      <c r="S14" s="61"/>
-      <c r="T14" s="61"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
     </row>
     <row r="15" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
@@ -1587,16 +1587,16 @@
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
       <c r="M17" s="7"/>
@@ -1605,16 +1605,16 @@
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
       <c r="N18" s="22"/>
       <c r="O18" s="22"/>
       <c r="P18" s="23"/>
@@ -1623,16 +1623,16 @@
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="13"/>
@@ -1668,16 +1668,16 @@
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
       <c r="K22" s="17"/>
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
@@ -1688,32 +1688,32 @@
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
       <c r="P23" s="17"/>
     </row>
     <row r="24" spans="1:16" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
       <c r="P24" s="17"/>
     </row>
     <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1738,46 +1738,46 @@
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
     </row>
     <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="64" t="s">
+      <c r="B29" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C29" s="64"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="64"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
       <c r="K29" s="29"/>
       <c r="L29" s="29"/>
     </row>
@@ -1808,46 +1808,46 @@
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
     </row>
     <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="64" t="s">
+      <c r="B34" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="64"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="64"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
@@ -2573,7 +2573,7 @@
       <c r="H112" s="20"/>
       <c r="I112" s="20"/>
     </row>
-    <row r="113" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C113" s="20"/>
       <c r="D113" s="20"/>
       <c r="E113" s="20"/>
@@ -2582,7 +2582,7 @@
       <c r="H113" s="20"/>
       <c r="I113" s="20"/>
     </row>
-    <row r="114" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C114" s="20"/>
       <c r="D114" s="20"/>
       <c r="E114" s="20"/>
@@ -2591,7 +2591,7 @@
       <c r="H114" s="20"/>
       <c r="I114" s="20"/>
     </row>
-    <row r="115" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C115" s="20"/>
       <c r="D115" s="20"/>
       <c r="E115" s="20"/>
@@ -2600,7 +2600,7 @@
       <c r="H115" s="20"/>
       <c r="I115" s="20"/>
     </row>
-    <row r="116" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C116" s="20"/>
       <c r="D116" s="20"/>
       <c r="E116" s="20"/>
@@ -2609,7 +2609,7 @@
       <c r="H116" s="20"/>
       <c r="I116" s="20"/>
     </row>
-    <row r="117" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C117" s="20"/>
       <c r="D117" s="20"/>
       <c r="E117" s="20"/>
@@ -2618,7 +2618,7 @@
       <c r="H117" s="20"/>
       <c r="I117" s="20"/>
     </row>
-    <row r="118" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C118" s="20"/>
       <c r="D118" s="20"/>
       <c r="E118" s="20"/>
@@ -2627,7 +2627,7 @@
       <c r="H118" s="20"/>
       <c r="I118" s="20"/>
     </row>
-    <row r="119" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C119" s="20"/>
       <c r="D119" s="20"/>
       <c r="E119" s="20"/>
@@ -2636,7 +2636,7 @@
       <c r="H119" s="20"/>
       <c r="I119" s="20"/>
     </row>
-    <row r="120" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C120" s="20"/>
       <c r="D120" s="20"/>
       <c r="E120" s="20"/>
@@ -2645,7 +2645,7 @@
       <c r="H120" s="20"/>
       <c r="I120" s="20"/>
     </row>
-    <row r="121" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C121" s="20"/>
       <c r="D121" s="20"/>
       <c r="E121" s="20"/>
@@ -2654,7 +2654,7 @@
       <c r="H121" s="20"/>
       <c r="I121" s="20"/>
     </row>
-    <row r="122" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C122" s="20"/>
       <c r="D122" s="20"/>
       <c r="E122" s="20"/>
@@ -2663,92 +2663,76 @@
       <c r="H122" s="20"/>
       <c r="I122" s="20"/>
     </row>
-    <row r="123" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="5"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="16"/>
-      <c r="E123" s="16"/>
-      <c r="F123" s="16"/>
-      <c r="G123" s="16"/>
-      <c r="H123" s="16"/>
-    </row>
-    <row r="124" spans="1:9" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="35" t="s">
+    <row r="123" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C123" s="20"/>
+      <c r="D123" s="20"/>
+      <c r="E123" s="20"/>
+      <c r="F123" s="20"/>
+      <c r="G123" s="20"/>
+      <c r="H123" s="20"/>
+      <c r="I123" s="20"/>
+    </row>
+    <row r="124" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C124" s="20"/>
+      <c r="D124" s="20"/>
+      <c r="E124" s="20"/>
+      <c r="F124" s="20"/>
+      <c r="G124" s="20"/>
+      <c r="H124" s="20"/>
+      <c r="I124" s="20"/>
+    </row>
+    <row r="125" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C125" s="20"/>
+      <c r="D125" s="20"/>
+      <c r="E125" s="20"/>
+      <c r="F125" s="20"/>
+      <c r="G125" s="20"/>
+      <c r="H125" s="20"/>
+      <c r="I125" s="20"/>
+    </row>
+    <row r="126" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C126" s="20"/>
+      <c r="D126" s="20"/>
+      <c r="E126" s="20"/>
+      <c r="F126" s="20"/>
+      <c r="G126" s="20"/>
+      <c r="H126" s="20"/>
+      <c r="I126" s="20"/>
+    </row>
+    <row r="127" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C127" s="20"/>
+      <c r="D127" s="20"/>
+      <c r="E127" s="20"/>
+      <c r="F127" s="20"/>
+      <c r="G127" s="20"/>
+      <c r="H127" s="20"/>
+      <c r="I127" s="20"/>
+    </row>
+    <row r="128" spans="3:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C128" s="20"/>
+      <c r="D128" s="20"/>
+      <c r="E128" s="20"/>
+      <c r="F128" s="20"/>
+      <c r="G128" s="20"/>
+      <c r="H128" s="20"/>
+      <c r="I128" s="20"/>
+    </row>
+    <row r="129" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="16"/>
+      <c r="E129" s="16"/>
+      <c r="F129" s="16"/>
+      <c r="G129" s="16"/>
+      <c r="H129" s="16"/>
+    </row>
+    <row r="130" spans="1:9" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B124" s="34" t="s">
+      <c r="B130" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="D124" s="16"/>
-      <c r="E124" s="16"/>
-      <c r="F124" s="16"/>
-      <c r="G124" s="16"/>
-      <c r="H124" s="16"/>
-      <c r="I124" s="33"/>
-    </row>
-    <row r="125" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="B125" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="D125" s="16"/>
-      <c r="E125" s="16"/>
-      <c r="F125" s="16"/>
-      <c r="G125" s="16"/>
-      <c r="H125" s="16"/>
-      <c r="I125" s="33"/>
-    </row>
-    <row r="126" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="35"/>
-      <c r="B126" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="C126" s="48"/>
-      <c r="D126" s="48"/>
-      <c r="E126" s="48"/>
-      <c r="F126" s="48"/>
-      <c r="G126" s="48"/>
-      <c r="H126" s="48"/>
-      <c r="I126" s="48"/>
-    </row>
-    <row r="127" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="35"/>
-      <c r="B127" s="48"/>
-      <c r="C127" s="48"/>
-      <c r="D127" s="48"/>
-      <c r="E127" s="48"/>
-      <c r="F127" s="48"/>
-      <c r="G127" s="48"/>
-      <c r="H127" s="48"/>
-      <c r="I127" s="48"/>
-    </row>
-    <row r="128" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="35"/>
-      <c r="B128" s="48"/>
-      <c r="C128" s="48"/>
-      <c r="D128" s="48"/>
-      <c r="E128" s="48"/>
-      <c r="F128" s="48"/>
-      <c r="G128" s="48"/>
-      <c r="H128" s="48"/>
-      <c r="I128" s="48"/>
-    </row>
-    <row r="129" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="35"/>
-      <c r="B129" s="48"/>
-      <c r="C129" s="48"/>
-      <c r="D129" s="48"/>
-      <c r="E129" s="48"/>
-      <c r="F129" s="48"/>
-      <c r="G129" s="48"/>
-      <c r="H129" s="48"/>
-      <c r="I129" s="48"/>
-    </row>
-    <row r="130" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="35"/>
-      <c r="B130" s="34"/>
       <c r="D130" s="16"/>
       <c r="E130" s="16"/>
       <c r="F130" s="16"/>
@@ -2756,12 +2740,12 @@
       <c r="H130" s="16"/>
       <c r="I130" s="33"/>
     </row>
-    <row r="131" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="34">
-        <v>3.2</v>
+    <row r="131" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="40" t="s">
+        <v>117</v>
       </c>
       <c r="B131" s="34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D131" s="16"/>
       <c r="E131" s="16"/>
@@ -2770,10 +2754,10 @@
       <c r="H131" s="16"/>
       <c r="I131" s="33"/>
     </row>
-    <row r="132" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="35"/>
       <c r="B132" s="48" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C132" s="48"/>
       <c r="D132" s="48"/>
@@ -2783,7 +2767,7 @@
       <c r="H132" s="48"/>
       <c r="I132" s="48"/>
     </row>
-    <row r="133" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="35"/>
       <c r="B133" s="48"/>
       <c r="C133" s="48"/>
@@ -2794,41 +2778,31 @@
       <c r="H133" s="48"/>
       <c r="I133" s="48"/>
     </row>
-    <row r="134" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B134" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D134" s="16"/>
-      <c r="E134" s="16"/>
-      <c r="F134" s="16"/>
-      <c r="G134" s="16"/>
-      <c r="H134" s="16"/>
-      <c r="I134" s="33"/>
-    </row>
-    <row r="135" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B135" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D135" s="16"/>
-      <c r="E135" s="16"/>
-      <c r="F135" s="16"/>
-      <c r="G135" s="16"/>
-      <c r="H135" s="16"/>
-      <c r="I135" s="33"/>
-    </row>
-    <row r="136" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B136" s="7" t="s">
-        <v>133</v>
-      </c>
+    <row r="134" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="35"/>
+      <c r="B134" s="48"/>
+      <c r="C134" s="48"/>
+      <c r="D134" s="48"/>
+      <c r="E134" s="48"/>
+      <c r="F134" s="48"/>
+      <c r="G134" s="48"/>
+      <c r="H134" s="48"/>
+      <c r="I134" s="48"/>
+    </row>
+    <row r="135" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="35"/>
+      <c r="B135" s="48"/>
+      <c r="C135" s="48"/>
+      <c r="D135" s="48"/>
+      <c r="E135" s="48"/>
+      <c r="F135" s="48"/>
+      <c r="G135" s="48"/>
+      <c r="H135" s="48"/>
+      <c r="I135" s="48"/>
+    </row>
+    <row r="136" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="35"/>
+      <c r="B136" s="34"/>
       <c r="D136" s="16"/>
       <c r="E136" s="16"/>
       <c r="F136" s="16"/>
@@ -2836,9 +2810,13 @@
       <c r="H136" s="16"/>
       <c r="I136" s="33"/>
     </row>
-    <row r="137" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="10"/>
-      <c r="B137" s="7"/>
+    <row r="137" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="34">
+        <v>3.2</v>
+      </c>
+      <c r="B137" s="34" t="s">
+        <v>128</v>
+      </c>
       <c r="D137" s="16"/>
       <c r="E137" s="16"/>
       <c r="F137" s="16"/>
@@ -2846,32 +2824,36 @@
       <c r="H137" s="16"/>
       <c r="I137" s="33"/>
     </row>
-    <row r="138" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="10"/>
-      <c r="B138" s="7"/>
-      <c r="D138" s="16"/>
-      <c r="E138" s="16"/>
-      <c r="F138" s="16"/>
-      <c r="G138" s="16"/>
-      <c r="H138" s="16"/>
-      <c r="I138" s="33"/>
-    </row>
-    <row r="139" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="35"/>
+      <c r="B138" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="C138" s="48"/>
+      <c r="D138" s="48"/>
+      <c r="E138" s="48"/>
+      <c r="F138" s="48"/>
+      <c r="G138" s="48"/>
+      <c r="H138" s="48"/>
+      <c r="I138" s="48"/>
+    </row>
+    <row r="139" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="35"/>
-      <c r="B139" s="34"/>
-      <c r="D139" s="16"/>
-      <c r="E139" s="16"/>
-      <c r="F139" s="16"/>
-      <c r="G139" s="16"/>
-      <c r="H139" s="16"/>
-      <c r="I139" s="33"/>
-    </row>
-    <row r="140" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="34">
-        <v>3.3</v>
-      </c>
-      <c r="B140" s="34" t="s">
-        <v>129</v>
+      <c r="B139" s="48"/>
+      <c r="C139" s="48"/>
+      <c r="D139" s="48"/>
+      <c r="E139" s="48"/>
+      <c r="F139" s="48"/>
+      <c r="G139" s="48"/>
+      <c r="H139" s="48"/>
+      <c r="I139" s="48"/>
+    </row>
+    <row r="140" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="D140" s="16"/>
       <c r="E140" s="16"/>
@@ -2880,125 +2862,105 @@
       <c r="H140" s="16"/>
       <c r="I140" s="33"/>
     </row>
-    <row r="141" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="34"/>
-      <c r="B141" s="52" t="s">
+    <row r="141" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D141" s="16"/>
+      <c r="E141" s="16"/>
+      <c r="F141" s="16"/>
+      <c r="G141" s="16"/>
+      <c r="H141" s="16"/>
+      <c r="I141" s="33"/>
+    </row>
+    <row r="142" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D142" s="16"/>
+      <c r="E142" s="16"/>
+      <c r="F142" s="16"/>
+      <c r="G142" s="16"/>
+      <c r="H142" s="16"/>
+      <c r="I142" s="33"/>
+    </row>
+    <row r="143" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="10"/>
+      <c r="B143" s="7"/>
+      <c r="D143" s="16"/>
+      <c r="E143" s="16"/>
+      <c r="F143" s="16"/>
+      <c r="G143" s="16"/>
+      <c r="H143" s="16"/>
+      <c r="I143" s="33"/>
+    </row>
+    <row r="144" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="10"/>
+      <c r="B144" s="7"/>
+      <c r="D144" s="16"/>
+      <c r="E144" s="16"/>
+      <c r="F144" s="16"/>
+      <c r="G144" s="16"/>
+      <c r="H144" s="16"/>
+      <c r="I144" s="33"/>
+    </row>
+    <row r="145" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="35"/>
+      <c r="B145" s="34"/>
+      <c r="D145" s="16"/>
+      <c r="E145" s="16"/>
+      <c r="F145" s="16"/>
+      <c r="G145" s="16"/>
+      <c r="H145" s="16"/>
+      <c r="I145" s="33"/>
+    </row>
+    <row r="146" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="34">
+        <v>3.3</v>
+      </c>
+      <c r="B146" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D146" s="16"/>
+      <c r="E146" s="16"/>
+      <c r="F146" s="16"/>
+      <c r="G146" s="16"/>
+      <c r="H146" s="16"/>
+      <c r="I146" s="33"/>
+    </row>
+    <row r="147" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="34"/>
+      <c r="B147" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="C141" s="52"/>
-      <c r="D141" s="52"/>
-      <c r="E141" s="52"/>
-      <c r="F141" s="52"/>
-      <c r="G141" s="52"/>
-      <c r="H141" s="52"/>
-      <c r="I141" s="52"/>
-      <c r="Q141" s="34"/>
-    </row>
-    <row r="142" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="10" t="str">
-        <f t="shared" ref="A142:A151" si="3">IF(B142&lt;&gt;"","•","")</f>
-        <v/>
-      </c>
-      <c r="B142" s="5" t="str" cm="1">
-        <f t="array" ref="B142">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
-        <v/>
-      </c>
-      <c r="C142" s="7"/>
-      <c r="D142" s="9"/>
-      <c r="E142" s="7"/>
-      <c r="F142" s="9"/>
-      <c r="Q142" s="10"/>
-    </row>
-    <row r="143" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B143" s="5" t="str" cm="1">
-        <f t="array" ref="B143">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
-        <v/>
-      </c>
-      <c r="C143" s="7"/>
-      <c r="D143" s="23"/>
-      <c r="E143" s="22"/>
-      <c r="F143" s="23"/>
-      <c r="Q143" s="10"/>
-    </row>
-    <row r="144" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B144" s="5" t="str" cm="1">
-        <f t="array" ref="B144">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
-        <v/>
-      </c>
-      <c r="C144" s="7"/>
-      <c r="D144" s="23"/>
-      <c r="E144" s="22"/>
-      <c r="F144" s="23"/>
-      <c r="Q144" s="10"/>
-      <c r="R144" s="7"/>
-    </row>
-    <row r="145" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B145" s="5" t="str" cm="1">
-        <f t="array" ref="B145">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
-        <v/>
-      </c>
-      <c r="C145" s="12"/>
-      <c r="D145" s="7"/>
-      <c r="E145" s="22"/>
-      <c r="F145" s="22"/>
-      <c r="Q145" s="10"/>
-    </row>
-    <row r="146" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B146" s="5" t="str" cm="1">
-        <f t="array" ref="B146">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
-        <v/>
-      </c>
-      <c r="C146" s="12"/>
-      <c r="D146" s="12"/>
-      <c r="E146" s="12"/>
-      <c r="F146" s="12"/>
-      <c r="Q146" s="10"/>
-    </row>
-    <row r="147" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B147" s="5" t="str" cm="1">
-        <f t="array" ref="B147">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
-        <v/>
-      </c>
-      <c r="C147"/>
-      <c r="D147"/>
-      <c r="E147"/>
-      <c r="F147"/>
-      <c r="Q147" s="10"/>
-      <c r="R147" s="7"/>
+      <c r="C147" s="46"/>
+      <c r="D147" s="46"/>
+      <c r="E147" s="46"/>
+      <c r="F147" s="46"/>
+      <c r="G147" s="46"/>
+      <c r="H147" s="46"/>
+      <c r="I147" s="46"/>
+      <c r="Q147" s="34"/>
     </row>
     <row r="148" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A148:A157" si="3">IF(B148&lt;&gt;"","•","")</f>
         <v/>
       </c>
       <c r="B148" s="5" t="str" cm="1">
         <f t="array" ref="B148">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
         <v/>
       </c>
-      <c r="C148"/>
-      <c r="D148"/>
-      <c r="E148" s="11"/>
-      <c r="F148"/>
+      <c r="C148" s="7"/>
+      <c r="D148" s="9"/>
+      <c r="E148" s="7"/>
+      <c r="F148" s="9"/>
       <c r="Q148" s="10"/>
     </row>
     <row r="149" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3010,6 +2972,10 @@
         <f t="array" ref="B149">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
         <v/>
       </c>
+      <c r="C149" s="7"/>
+      <c r="D149" s="23"/>
+      <c r="E149" s="22"/>
+      <c r="F149" s="23"/>
       <c r="Q149" s="10"/>
     </row>
     <row r="150" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3021,11 +2987,12 @@
         <f t="array" ref="B150">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
         <v/>
       </c>
-      <c r="C150"/>
-      <c r="D150"/>
-      <c r="E150"/>
-      <c r="F150"/>
+      <c r="C150" s="7"/>
+      <c r="D150" s="23"/>
+      <c r="E150" s="22"/>
+      <c r="F150" s="23"/>
       <c r="Q150" s="10"/>
+      <c r="R150" s="7"/>
     </row>
     <row r="151" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="10" t="str">
@@ -3036,306 +3003,319 @@
         <f t="array" ref="B151">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
         <v/>
       </c>
-      <c r="C151"/>
-      <c r="D151"/>
-      <c r="E151"/>
-      <c r="F151"/>
+      <c r="C151" s="12"/>
+      <c r="D151" s="7"/>
+      <c r="E151" s="22"/>
+      <c r="F151" s="22"/>
       <c r="Q151" s="10"/>
     </row>
     <row r="152" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M152" s="5" t="str">
-        <f t="array" ref="M152">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
+      <c r="A152" s="10" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="N152" s="9"/>
-      <c r="O152" s="7"/>
-      <c r="P152" s="9"/>
-    </row>
-    <row r="153" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="34">
+      <c r="B152" s="5" t="str" cm="1">
+        <f t="array" ref="B152">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
+        <v/>
+      </c>
+      <c r="C152" s="12"/>
+      <c r="D152" s="12"/>
+      <c r="E152" s="12"/>
+      <c r="F152" s="12"/>
+      <c r="Q152" s="10"/>
+    </row>
+    <row r="153" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B153" s="5" t="str" cm="1">
+        <f t="array" ref="B153">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
+        <v/>
+      </c>
+      <c r="C153"/>
+      <c r="D153"/>
+      <c r="E153"/>
+      <c r="F153"/>
+      <c r="Q153" s="10"/>
+      <c r="R153" s="7"/>
+    </row>
+    <row r="154" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B154" s="5" t="str" cm="1">
+        <f t="array" ref="B154">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
+        <v/>
+      </c>
+      <c r="C154"/>
+      <c r="D154"/>
+      <c r="E154" s="11"/>
+      <c r="F154"/>
+      <c r="Q154" s="10"/>
+    </row>
+    <row r="155" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B155" s="5" t="str" cm="1">
+        <f t="array" ref="B155">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
+        <v/>
+      </c>
+      <c r="Q155" s="10"/>
+    </row>
+    <row r="156" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B156" s="5" t="str" cm="1">
+        <f t="array" ref="B156">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
+        <v/>
+      </c>
+      <c r="C156"/>
+      <c r="D156"/>
+      <c r="E156"/>
+      <c r="F156"/>
+      <c r="Q156" s="10"/>
+    </row>
+    <row r="157" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B157" s="5" t="str" cm="1">
+        <f t="array" ref="B157">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
+        <v/>
+      </c>
+      <c r="C157"/>
+      <c r="D157"/>
+      <c r="E157"/>
+      <c r="F157"/>
+      <c r="Q157" s="10"/>
+    </row>
+    <row r="158" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M158" s="5" t="str">
+        <f t="array" ref="M158">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
+        <v/>
+      </c>
+      <c r="N158" s="9"/>
+      <c r="O158" s="7"/>
+      <c r="P158" s="9"/>
+    </row>
+    <row r="159" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="34">
         <v>3.4</v>
       </c>
-      <c r="B153" s="34" t="s">
+      <c r="B159" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="M153" s="5" t="str">
-        <f t="array" ref="M153">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
+      <c r="M159" s="5" t="str">
+        <f t="array" ref="M159">IFERROR(INDEX(#REF!,SMALL(IF(#REF!=#REF!,ROW(#REF!)-ROW(#REF!)+1),ROWS(#REF!))),"")</f>
         <v/>
       </c>
-      <c r="N153" s="23"/>
-      <c r="O153" s="22"/>
-      <c r="P153" s="23"/>
-      <c r="Q153" s="5"/>
-    </row>
-    <row r="154" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="34"/>
-      <c r="B154" s="49" t="s">
+      <c r="N159" s="23"/>
+      <c r="O159" s="22"/>
+      <c r="P159" s="23"/>
+      <c r="Q159" s="5"/>
+    </row>
+    <row r="160" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="34"/>
+      <c r="B160" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C154" s="49"/>
-      <c r="D154" s="49"/>
-      <c r="E154" s="49"/>
-      <c r="F154" s="49"/>
-      <c r="G154" s="49"/>
-      <c r="H154" s="49"/>
-      <c r="I154" s="49"/>
-      <c r="M154" s="7"/>
-      <c r="N154" s="23"/>
-      <c r="O154" s="22"/>
-      <c r="P154" s="23"/>
-      <c r="Q154" s="5"/>
-    </row>
-    <row r="155" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="34"/>
-      <c r="B155" t="s">
+      <c r="C160" s="47"/>
+      <c r="D160" s="47"/>
+      <c r="E160" s="47"/>
+      <c r="F160" s="47"/>
+      <c r="G160" s="47"/>
+      <c r="H160" s="47"/>
+      <c r="I160" s="47"/>
+      <c r="M160" s="7"/>
+      <c r="N160" s="23"/>
+      <c r="O160" s="22"/>
+      <c r="P160" s="23"/>
+      <c r="Q160" s="5"/>
+    </row>
+    <row r="161" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="34"/>
+      <c r="B161" t="s">
         <v>9</v>
       </c>
-      <c r="E155" s="38" t="s">
+      <c r="E161" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="M155" s="12"/>
-      <c r="N155" s="7"/>
-      <c r="O155" s="22"/>
-      <c r="P155" s="22"/>
-      <c r="Q155" s="5"/>
-    </row>
-    <row r="156" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B156" t="s">
+      <c r="M161" s="12"/>
+      <c r="N161" s="7"/>
+      <c r="O161" s="22"/>
+      <c r="P161" s="22"/>
+      <c r="Q161" s="5"/>
+    </row>
+    <row r="162" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
         <v>12</v>
       </c>
-      <c r="E156" s="5"/>
-      <c r="M156" s="12"/>
-      <c r="N156" s="12"/>
-      <c r="O156" s="12"/>
-      <c r="P156" s="12"/>
-      <c r="Q156" s="5"/>
-    </row>
-    <row r="157" spans="1:18" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157"/>
-      <c r="B157" s="5"/>
-      <c r="C157" s="5"/>
-      <c r="D157" s="16"/>
-      <c r="E157" s="16"/>
-      <c r="F157" s="16"/>
-      <c r="G157" s="16"/>
-      <c r="H157" s="16"/>
-      <c r="I157"/>
-      <c r="M157" s="5"/>
-      <c r="N157" s="5"/>
-      <c r="O157"/>
-      <c r="P157"/>
-      <c r="Q157" s="5"/>
-    </row>
-    <row r="158" spans="1:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="35" t="s">
+      <c r="E162" s="5"/>
+      <c r="M162" s="12"/>
+      <c r="N162" s="12"/>
+      <c r="O162" s="12"/>
+      <c r="P162" s="12"/>
+      <c r="Q162" s="5"/>
+    </row>
+    <row r="163" spans="1:17" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163"/>
+      <c r="B163" s="5"/>
+      <c r="C163" s="5"/>
+      <c r="D163" s="16"/>
+      <c r="E163" s="16"/>
+      <c r="F163" s="16"/>
+      <c r="G163" s="16"/>
+      <c r="H163" s="16"/>
+      <c r="I163"/>
+      <c r="M163" s="5"/>
+      <c r="N163" s="5"/>
+      <c r="O163"/>
+      <c r="P163"/>
+      <c r="Q163" s="5"/>
+    </row>
+    <row r="164" spans="1:17" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B158" s="34" t="s">
+      <c r="B164" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D158" s="16"/>
-      <c r="E158" s="16"/>
-      <c r="F158" s="16"/>
-      <c r="G158" s="16"/>
-      <c r="H158" s="16"/>
-      <c r="I158" s="33"/>
-      <c r="M158"/>
-      <c r="N158"/>
-      <c r="O158" s="11"/>
-      <c r="P158"/>
-    </row>
-    <row r="159" spans="1:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="52" t="s">
+      <c r="D164" s="16"/>
+      <c r="E164" s="16"/>
+      <c r="F164" s="16"/>
+      <c r="G164" s="16"/>
+      <c r="H164" s="16"/>
+      <c r="I164" s="33"/>
+      <c r="M164"/>
+      <c r="N164"/>
+      <c r="O164" s="11"/>
+      <c r="P164"/>
+    </row>
+    <row r="165" spans="1:17" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B165" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="C159" s="52"/>
-      <c r="D159" s="52"/>
-      <c r="E159" s="52"/>
-      <c r="F159" s="52"/>
-      <c r="G159" s="52"/>
-      <c r="H159" s="52"/>
-      <c r="I159" s="52"/>
-      <c r="M159"/>
-      <c r="N159"/>
-    </row>
-    <row r="160" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="28" t="s">
+      <c r="C165" s="46"/>
+      <c r="D165" s="46"/>
+      <c r="E165" s="46"/>
+      <c r="F165" s="46"/>
+      <c r="G165" s="46"/>
+      <c r="H165" s="46"/>
+      <c r="I165" s="46"/>
+      <c r="M165"/>
+      <c r="N165"/>
+    </row>
+    <row r="166" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B166" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C160" s="28"/>
-      <c r="D160" s="50" t="s">
+      <c r="C166" s="28"/>
+      <c r="D166" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="E160" s="50"/>
-      <c r="F160" s="50" t="s">
+      <c r="E166" s="57"/>
+      <c r="F166" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="G160" s="50"/>
-      <c r="H160" s="9"/>
-      <c r="Q160" s="5"/>
-    </row>
-    <row r="161" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B161" s="28" t="s">
+      <c r="G166" s="57"/>
+      <c r="H166" s="9"/>
+      <c r="Q166" s="5"/>
+    </row>
+    <row r="167" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B167" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C161" s="28"/>
-      <c r="D161" s="50" t="s">
+      <c r="C167" s="28"/>
+      <c r="D167" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="E161" s="50"/>
-      <c r="F161" s="51">
+      <c r="E167" s="57"/>
+      <c r="F167" s="58">
         <v>10000000</v>
       </c>
-      <c r="G161" s="51"/>
-      <c r="H161" s="23"/>
-      <c r="I161" s="7"/>
-      <c r="M161" s="5"/>
-      <c r="N161" s="5"/>
-      <c r="O161" s="5"/>
-      <c r="P161" s="5"/>
-      <c r="Q161" s="5"/>
-    </row>
-    <row r="162" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="28" t="s">
+      <c r="G167" s="58"/>
+      <c r="H167" s="23"/>
+      <c r="I167" s="7"/>
+      <c r="M167" s="5"/>
+      <c r="N167" s="5"/>
+      <c r="O167" s="5"/>
+      <c r="P167" s="5"/>
+      <c r="Q167" s="5"/>
+    </row>
+    <row r="168" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B168" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C162" s="28"/>
-      <c r="D162" s="50" t="s">
+      <c r="C168" s="28"/>
+      <c r="D168" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="E162" s="50"/>
-      <c r="F162" s="51">
+      <c r="E168" s="57"/>
+      <c r="F168" s="58">
         <v>20000000</v>
       </c>
-      <c r="G162" s="51"/>
-      <c r="H162" s="23"/>
-      <c r="M162" s="9"/>
-    </row>
-    <row r="163" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="12" t="s">
+      <c r="G168" s="58"/>
+      <c r="H168" s="23"/>
+      <c r="M168" s="9"/>
+    </row>
+    <row r="169" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B169" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C163" s="12"/>
-      <c r="D163" s="12"/>
-      <c r="E163" s="7"/>
-      <c r="F163" s="22"/>
-      <c r="G163" s="22"/>
-      <c r="H163" s="23"/>
-      <c r="M163" s="23"/>
-    </row>
-    <row r="164" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="12"/>
-      <c r="C164" s="12"/>
-      <c r="D164" s="12"/>
-      <c r="E164" s="12"/>
-      <c r="F164" s="12"/>
-      <c r="G164" s="12"/>
-      <c r="H164" s="12"/>
-      <c r="I164" s="12"/>
-      <c r="M164" s="23"/>
-    </row>
-    <row r="165" spans="1:17" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="B165" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C165" s="36"/>
-      <c r="I165" s="33"/>
-      <c r="M165" s="22"/>
-    </row>
-    <row r="166" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="1"/>
-      <c r="B166" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="C166" s="48"/>
-      <c r="D166" s="48"/>
-      <c r="E166" s="48"/>
-      <c r="F166" s="48"/>
-      <c r="G166" s="48"/>
-      <c r="H166" s="48"/>
-      <c r="I166" s="48"/>
-      <c r="M166" s="12"/>
-    </row>
-    <row r="167" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="1"/>
-      <c r="B167" s="48"/>
-      <c r="C167" s="48"/>
-      <c r="D167" s="48"/>
-      <c r="E167" s="48"/>
-      <c r="F167" s="48"/>
-      <c r="G167" s="48"/>
-      <c r="H167" s="48"/>
-      <c r="I167" s="48"/>
-    </row>
-    <row r="168" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="1"/>
-      <c r="B168" s="48"/>
-      <c r="C168" s="48"/>
-      <c r="D168" s="48"/>
-      <c r="E168" s="48"/>
-      <c r="F168" s="48"/>
-      <c r="G168" s="48"/>
-      <c r="H168" s="48"/>
-      <c r="I168" s="48"/>
-    </row>
-    <row r="169" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="1"/>
-      <c r="B169" s="48"/>
-      <c r="C169" s="48"/>
-      <c r="D169" s="48"/>
-      <c r="E169" s="48"/>
-      <c r="F169" s="48"/>
-      <c r="G169" s="48"/>
-      <c r="H169" s="48"/>
-      <c r="I169" s="48"/>
-      <c r="M169" s="5"/>
+      <c r="C169" s="12"/>
+      <c r="D169" s="12"/>
+      <c r="E169" s="7"/>
+      <c r="F169" s="22"/>
+      <c r="G169" s="22"/>
+      <c r="H169" s="23"/>
+      <c r="M169" s="23"/>
     </row>
     <row r="170" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="1"/>
-      <c r="B170" s="13"/>
-      <c r="C170" s="13"/>
-      <c r="D170" s="13"/>
-      <c r="E170" s="13"/>
-      <c r="F170" s="13"/>
-      <c r="G170" s="13"/>
-      <c r="H170" s="13"/>
-      <c r="I170" s="13"/>
+      <c r="B170" s="12"/>
+      <c r="C170" s="12"/>
+      <c r="D170" s="12"/>
+      <c r="E170" s="12"/>
+      <c r="F170" s="12"/>
+      <c r="G170" s="12"/>
+      <c r="H170" s="12"/>
+      <c r="I170" s="12"/>
+      <c r="M170" s="23"/>
     </row>
     <row r="171" spans="1:17" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="35" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="B171" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="D171" s="16"/>
-      <c r="E171" s="16"/>
-      <c r="F171" s="16"/>
-      <c r="G171" s="16"/>
-      <c r="H171" s="16"/>
+        <v>7</v>
+      </c>
+      <c r="C171" s="36"/>
       <c r="I171" s="33"/>
+      <c r="M171" s="22"/>
     </row>
     <row r="172" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C172" s="4"/>
-      <c r="E172" s="8"/>
-      <c r="F172" s="16"/>
-      <c r="G172" s="16"/>
-      <c r="H172" s="16"/>
-      <c r="I172" s="21"/>
+      <c r="A172" s="1"/>
+      <c r="B172" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="C172" s="48"/>
+      <c r="D172" s="48"/>
+      <c r="E172" s="48"/>
+      <c r="F172" s="48"/>
+      <c r="G172" s="48"/>
+      <c r="H172" s="48"/>
+      <c r="I172" s="48"/>
+      <c r="M172" s="12"/>
     </row>
     <row r="173" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B173" s="48" t="s">
-        <v>15</v>
-      </c>
+      <c r="A173" s="1"/>
+      <c r="B173" s="48"/>
       <c r="C173" s="48"/>
       <c r="D173" s="48"/>
       <c r="E173" s="48"/>
@@ -3344,7 +3324,8 @@
       <c r="H173" s="48"/>
       <c r="I173" s="48"/>
     </row>
-    <row r="174" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="1"/>
       <c r="B174" s="48"/>
       <c r="C174" s="48"/>
       <c r="D174" s="48"/>
@@ -3355,950 +3336,1069 @@
       <c r="I174" s="48"/>
     </row>
     <row r="175" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B175" s="53" t="s">
+      <c r="A175" s="1"/>
+      <c r="B175" s="48"/>
+      <c r="C175" s="48"/>
+      <c r="D175" s="48"/>
+      <c r="E175" s="48"/>
+      <c r="F175" s="48"/>
+      <c r="G175" s="48"/>
+      <c r="H175" s="48"/>
+      <c r="I175" s="48"/>
+      <c r="M175" s="5"/>
+    </row>
+    <row r="176" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1"/>
+      <c r="B176" s="13"/>
+      <c r="C176" s="13"/>
+      <c r="D176" s="13"/>
+      <c r="E176" s="13"/>
+      <c r="F176" s="13"/>
+      <c r="G176" s="13"/>
+      <c r="H176" s="13"/>
+      <c r="I176" s="13"/>
+    </row>
+    <row r="177" spans="1:9" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B177" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D177" s="16"/>
+      <c r="E177" s="16"/>
+      <c r="F177" s="16"/>
+      <c r="G177" s="16"/>
+      <c r="H177" s="16"/>
+      <c r="I177" s="33"/>
+    </row>
+    <row r="178" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C178" s="4"/>
+      <c r="E178" s="8"/>
+      <c r="F178" s="16"/>
+      <c r="G178" s="16"/>
+      <c r="H178" s="16"/>
+      <c r="I178" s="21"/>
+    </row>
+    <row r="179" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B179" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C179" s="48"/>
+      <c r="D179" s="48"/>
+      <c r="E179" s="48"/>
+      <c r="F179" s="48"/>
+      <c r="G179" s="48"/>
+      <c r="H179" s="48"/>
+      <c r="I179" s="48"/>
+    </row>
+    <row r="180" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B180" s="48"/>
+      <c r="C180" s="48"/>
+      <c r="D180" s="48"/>
+      <c r="E180" s="48"/>
+      <c r="F180" s="48"/>
+      <c r="G180" s="48"/>
+      <c r="H180" s="48"/>
+      <c r="I180" s="48"/>
+    </row>
+    <row r="181" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B181" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="C175" s="54"/>
-      <c r="D175" s="54"/>
-      <c r="E175" s="55"/>
-      <c r="F175" s="41" t="s">
+      <c r="C181" s="60"/>
+      <c r="D181" s="60"/>
+      <c r="E181" s="61"/>
+      <c r="F181" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="G175" s="41" t="s">
+      <c r="G181" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="H175" s="9"/>
-    </row>
-    <row r="176" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="56"/>
-      <c r="C176" s="57"/>
-      <c r="D176" s="57"/>
-      <c r="E176" s="58"/>
-      <c r="F176" s="31"/>
-      <c r="G176" s="31"/>
-      <c r="H176" s="23"/>
-      <c r="I176" s="7"/>
-    </row>
-    <row r="177" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B177" s="56"/>
-      <c r="C177" s="57"/>
-      <c r="D177" s="57"/>
-      <c r="E177" s="58"/>
-      <c r="F177" s="31"/>
-      <c r="G177" s="31"/>
-      <c r="H177" s="23"/>
-      <c r="I177" s="7"/>
-    </row>
-    <row r="178" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B178" s="56"/>
-      <c r="C178" s="57"/>
-      <c r="D178" s="57"/>
-      <c r="E178" s="58"/>
-      <c r="F178" s="31"/>
-      <c r="G178" s="31"/>
-      <c r="H178" s="23"/>
-      <c r="I178" s="7"/>
-    </row>
-    <row r="179" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C179" s="47" t="s">
+      <c r="H181" s="9"/>
+    </row>
+    <row r="182" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B182" s="62"/>
+      <c r="C182" s="63"/>
+      <c r="D182" s="63"/>
+      <c r="E182" s="64"/>
+      <c r="F182" s="31"/>
+      <c r="G182" s="31"/>
+      <c r="H182" s="23"/>
+      <c r="I182" s="7"/>
+    </row>
+    <row r="183" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B183" s="62"/>
+      <c r="C183" s="63"/>
+      <c r="D183" s="63"/>
+      <c r="E183" s="64"/>
+      <c r="F183" s="31"/>
+      <c r="G183" s="31"/>
+      <c r="H183" s="23"/>
+      <c r="I183" s="7"/>
+    </row>
+    <row r="184" spans="1:9" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B184" s="62"/>
+      <c r="C184" s="63"/>
+      <c r="D184" s="63"/>
+      <c r="E184" s="64"/>
+      <c r="F184" s="31"/>
+      <c r="G184" s="31"/>
+      <c r="H184" s="23"/>
+      <c r="I184" s="7"/>
+    </row>
+    <row r="185" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C185" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="D179" s="47"/>
-      <c r="E179" s="47"/>
-      <c r="F179" s="42">
-        <f>SUM(F176:F178)</f>
+      <c r="D185" s="56"/>
+      <c r="E185" s="56"/>
+      <c r="F185" s="42">
+        <f>SUM(F182:F184)</f>
         <v>0</v>
       </c>
-      <c r="G179" s="42">
-        <f>SUM(G176:G178)</f>
+      <c r="G185" s="42">
+        <f>SUM(G182:G184)</f>
         <v>0</v>
       </c>
-      <c r="H179" s="23"/>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C180" s="43"/>
-      <c r="D180" s="43"/>
-      <c r="E180" s="43"/>
-      <c r="F180" s="42"/>
-      <c r="G180" s="42"/>
-      <c r="H180" s="23"/>
-    </row>
-    <row r="181" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="21" t="s">
+      <c r="H185" s="23"/>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C186" s="43"/>
+      <c r="D186" s="43"/>
+      <c r="E186" s="43"/>
+      <c r="F186" s="42"/>
+      <c r="G186" s="42"/>
+      <c r="H186" s="23"/>
+    </row>
+    <row r="187" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="B181" s="2" t="s">
+      <c r="B187" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C181" s="12"/>
-      <c r="D181" s="12"/>
-      <c r="E181" s="7"/>
-      <c r="F181" s="22"/>
-      <c r="G181" s="22"/>
-      <c r="H181" s="23"/>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B182" s="48" t="s">
+      <c r="C187" s="12"/>
+      <c r="D187" s="12"/>
+      <c r="E187" s="7"/>
+      <c r="F187" s="22"/>
+      <c r="G187" s="22"/>
+      <c r="H187" s="23"/>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B188" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C182" s="48"/>
-      <c r="D182" s="48"/>
-      <c r="E182" s="48"/>
-      <c r="F182" s="48"/>
-      <c r="G182" s="48"/>
-      <c r="H182" s="48"/>
-      <c r="I182" s="48"/>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A183" s="21"/>
-      <c r="B183" s="48"/>
-      <c r="C183" s="48"/>
-      <c r="D183" s="48"/>
-      <c r="E183" s="48"/>
-      <c r="F183" s="48"/>
-      <c r="G183" s="48"/>
-      <c r="H183" s="48"/>
-      <c r="I183" s="48"/>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A184" s="21"/>
-      <c r="B184" s="48"/>
-      <c r="C184" s="48"/>
-      <c r="D184" s="48"/>
-      <c r="E184" s="48"/>
-      <c r="F184" s="48"/>
-      <c r="G184" s="48"/>
-      <c r="H184" s="48"/>
-      <c r="I184" s="48"/>
-    </row>
-    <row r="185" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B185" t="s">
+      <c r="C188" s="48"/>
+      <c r="D188" s="48"/>
+      <c r="E188" s="48"/>
+      <c r="F188" s="48"/>
+      <c r="G188" s="48"/>
+      <c r="H188" s="48"/>
+      <c r="I188" s="48"/>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A189" s="21"/>
+      <c r="B189" s="48"/>
+      <c r="C189" s="48"/>
+      <c r="D189" s="48"/>
+      <c r="E189" s="48"/>
+      <c r="F189" s="48"/>
+      <c r="G189" s="48"/>
+      <c r="H189" s="48"/>
+      <c r="I189" s="48"/>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A190" s="21"/>
+      <c r="B190" s="48"/>
+      <c r="C190" s="48"/>
+      <c r="D190" s="48"/>
+      <c r="E190" s="48"/>
+      <c r="F190" s="48"/>
+      <c r="G190" s="48"/>
+      <c r="H190" s="48"/>
+      <c r="I190" s="48"/>
+    </row>
+    <row r="191" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B191" t="s">
         <v>16</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D191" t="s">
         <v>10</v>
       </c>
-      <c r="E185" s="25">
+      <c r="E191" s="25">
         <v>280</v>
       </c>
-      <c r="F185" s="25" t="s">
+      <c r="F191" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="H185" s="24"/>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B186" t="s">
+      <c r="H191" s="24"/>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B192" t="s">
         <v>135</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D192" t="s">
         <v>10</v>
       </c>
-      <c r="E186" s="25">
+      <c r="E192" s="25">
         <v>150</v>
       </c>
-      <c r="F186" s="25" t="s">
+      <c r="F192" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="H186" s="24"/>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B187" t="s">
+      <c r="H192" s="24"/>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
         <v>136</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D193" t="s">
         <v>10</v>
       </c>
-      <c r="E187" s="25">
+      <c r="E193" s="25">
         <v>450</v>
       </c>
-      <c r="F187" s="25" t="s">
+      <c r="F193" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="H187" s="24"/>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E188" s="25"/>
-      <c r="F188" s="25"/>
-      <c r="H188" s="24"/>
-    </row>
-    <row r="189" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="21" t="s">
+      <c r="H193" s="24"/>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E194" s="25"/>
+      <c r="F194" s="25"/>
+      <c r="H194" s="24"/>
+    </row>
+    <row r="195" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="B189" s="2" t="s">
+      <c r="B195" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E189" s="25"/>
-      <c r="F189" s="25"/>
-      <c r="H189" s="24"/>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B190" s="7" t="s">
+      <c r="E195" s="25"/>
+      <c r="F195" s="25"/>
+      <c r="H195" s="24"/>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B196" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C190" s="43"/>
-      <c r="D190" s="43"/>
-      <c r="E190" s="43"/>
-      <c r="F190" s="42"/>
-      <c r="G190" s="42"/>
-      <c r="H190" s="23"/>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A191" s="17"/>
-      <c r="B191" s="17"/>
-      <c r="C191" s="17"/>
-      <c r="D191" s="17"/>
-      <c r="E191" s="17"/>
-      <c r="F191" s="17"/>
-      <c r="G191" s="17"/>
-      <c r="H191" s="17"/>
-      <c r="I191" s="17"/>
-    </row>
-    <row r="192" spans="1:9" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="35" t="s">
+      <c r="C196" s="43"/>
+      <c r="D196" s="43"/>
+      <c r="E196" s="43"/>
+      <c r="F196" s="42"/>
+      <c r="G196" s="42"/>
+      <c r="H196" s="23"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197" s="17"/>
+      <c r="B197" s="17"/>
+      <c r="C197" s="17"/>
+      <c r="D197" s="17"/>
+      <c r="E197" s="17"/>
+      <c r="F197" s="17"/>
+      <c r="G197" s="17"/>
+      <c r="H197" s="17"/>
+      <c r="I197" s="17"/>
+    </row>
+    <row r="198" spans="1:9" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B192" s="34" t="s">
+      <c r="B198" s="34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A193" s="21"/>
-      <c r="B193" s="2"/>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A194" s="21"/>
-      <c r="B194" s="2"/>
-      <c r="C194" s="1" t="s">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199" s="21"/>
+      <c r="B199" s="2"/>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200" s="21"/>
+      <c r="B200" s="2"/>
+      <c r="C200" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D194" s="1"/>
-      <c r="E194" s="1"/>
-      <c r="F194" s="1" t="s">
+      <c r="D200" s="1"/>
+      <c r="E200" s="1"/>
+      <c r="F200" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B195" s="12" t="s">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B201" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F195" t="s">
+      <c r="F201" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B196" s="12"/>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B197" s="12" t="s">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B202" s="12"/>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B203" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F197" t="s">
+      <c r="F203" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B198" s="12"/>
-      <c r="F198" t="s">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B204" s="12"/>
+      <c r="F204" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B199" s="12"/>
-      <c r="F199" t="s">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B205" s="12"/>
+      <c r="F205" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B200" s="12"/>
-      <c r="F200" t="s">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B206" s="12"/>
+      <c r="F206" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B201" s="12"/>
-      <c r="F201" s="2" t="s">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B207" s="12"/>
+      <c r="F207" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B202" s="12"/>
-      <c r="F202" t="s">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B208" s="12"/>
+      <c r="F208" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="203" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B203" s="12" t="s">
+    <row r="209" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B209" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B204" s="10"/>
-    </row>
-    <row r="205" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B205" s="10"/>
-    </row>
-    <row r="206" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B206" s="10"/>
-    </row>
-    <row r="207" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B207" s="10"/>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B208" s="10" t="s">
+    <row r="210" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B210" s="10"/>
+    </row>
+    <row r="211" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B211" s="10"/>
+    </row>
+    <row r="212" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B212" s="10"/>
+    </row>
+    <row r="213" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B213" s="10"/>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B214" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F208" s="59">
+      <c r="F214" s="55">
         <f ca="1">TODAY()</f>
-        <v>45224</v>
-      </c>
-      <c r="G208" s="59"/>
-    </row>
-    <row r="209" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="37" t="s">
+        <v>45226</v>
+      </c>
+      <c r="G214" s="55"/>
+    </row>
+    <row r="215" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A215" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="C209" s="6"/>
-      <c r="I209" s="21"/>
-    </row>
-    <row r="210" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="8">
+      <c r="C215" s="6"/>
+      <c r="I215" s="21"/>
+    </row>
+    <row r="216" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="8">
         <v>1</v>
       </c>
-      <c r="B210" s="46" t="s">
+      <c r="B216" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="C210" s="46"/>
-      <c r="D210" s="46"/>
-      <c r="E210" s="46"/>
-      <c r="F210" s="46"/>
-      <c r="G210" s="46"/>
-      <c r="H210" s="46"/>
-      <c r="I210" s="46"/>
-    </row>
-    <row r="211" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="8">
+      <c r="C216" s="54"/>
+      <c r="D216" s="54"/>
+      <c r="E216" s="54"/>
+      <c r="F216" s="54"/>
+      <c r="G216" s="54"/>
+      <c r="H216" s="54"/>
+      <c r="I216" s="54"/>
+    </row>
+    <row r="217" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A217" s="8">
         <v>2</v>
       </c>
-      <c r="B211" s="46" t="s">
+      <c r="B217" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="C211" s="46"/>
-      <c r="D211" s="46"/>
-      <c r="E211" s="46"/>
-      <c r="F211" s="46"/>
-      <c r="G211" s="46"/>
-      <c r="H211" s="46"/>
-      <c r="I211" s="46"/>
-    </row>
-    <row r="212" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="8">
+      <c r="C217" s="54"/>
+      <c r="D217" s="54"/>
+      <c r="E217" s="54"/>
+      <c r="F217" s="54"/>
+      <c r="G217" s="54"/>
+      <c r="H217" s="54"/>
+      <c r="I217" s="54"/>
+    </row>
+    <row r="218" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A218" s="8">
         <v>3</v>
       </c>
-      <c r="B212" s="46" t="s">
+      <c r="B218" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="C212" s="46"/>
-      <c r="D212" s="46"/>
-      <c r="E212" s="46"/>
-      <c r="F212" s="46"/>
-      <c r="G212" s="46"/>
-      <c r="H212" s="46"/>
-      <c r="I212" s="46"/>
-    </row>
-    <row r="213" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="8">
+      <c r="C218" s="54"/>
+      <c r="D218" s="54"/>
+      <c r="E218" s="54"/>
+      <c r="F218" s="54"/>
+      <c r="G218" s="54"/>
+      <c r="H218" s="54"/>
+      <c r="I218" s="54"/>
+    </row>
+    <row r="219" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="8">
         <v>4</v>
       </c>
-      <c r="B213" s="46" t="s">
+      <c r="B219" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="C213" s="46"/>
-      <c r="D213" s="46"/>
-      <c r="E213" s="46"/>
-      <c r="F213" s="46"/>
-      <c r="G213" s="46"/>
-      <c r="H213" s="46"/>
-      <c r="I213" s="46"/>
-    </row>
-    <row r="214" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="8">
+      <c r="C219" s="54"/>
+      <c r="D219" s="54"/>
+      <c r="E219" s="54"/>
+      <c r="F219" s="54"/>
+      <c r="G219" s="54"/>
+      <c r="H219" s="54"/>
+      <c r="I219" s="54"/>
+    </row>
+    <row r="220" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="8">
         <v>5</v>
       </c>
-      <c r="B214" s="46" t="s">
+      <c r="B220" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="C214" s="46"/>
-      <c r="D214" s="46"/>
-      <c r="E214" s="46"/>
-      <c r="F214" s="46"/>
-      <c r="G214" s="46"/>
-      <c r="H214" s="46"/>
-      <c r="I214" s="46"/>
-    </row>
-    <row r="215" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="8"/>
-      <c r="B215" s="46" t="s">
+      <c r="C220" s="54"/>
+      <c r="D220" s="54"/>
+      <c r="E220" s="54"/>
+      <c r="F220" s="54"/>
+      <c r="G220" s="54"/>
+      <c r="H220" s="54"/>
+      <c r="I220" s="54"/>
+    </row>
+    <row r="221" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="8"/>
+      <c r="B221" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="C215" s="46"/>
-      <c r="D215" s="46"/>
-      <c r="E215" s="46"/>
-      <c r="F215" s="46"/>
-      <c r="G215" s="46"/>
-      <c r="H215" s="46"/>
-      <c r="I215" s="46"/>
-    </row>
-    <row r="216" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="8"/>
-      <c r="B216" s="46" t="s">
+      <c r="C221" s="54"/>
+      <c r="D221" s="54"/>
+      <c r="E221" s="54"/>
+      <c r="F221" s="54"/>
+      <c r="G221" s="54"/>
+      <c r="H221" s="54"/>
+      <c r="I221" s="54"/>
+    </row>
+    <row r="222" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="8"/>
+      <c r="B222" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C216" s="46"/>
-      <c r="D216" s="46"/>
-      <c r="E216" s="46"/>
-      <c r="F216" s="46"/>
-      <c r="G216" s="46"/>
-      <c r="H216" s="46"/>
-      <c r="I216" s="46"/>
-    </row>
-    <row r="217" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A217" s="8"/>
-      <c r="B217" s="46" t="s">
+      <c r="C222" s="54"/>
+      <c r="D222" s="54"/>
+      <c r="E222" s="54"/>
+      <c r="F222" s="54"/>
+      <c r="G222" s="54"/>
+      <c r="H222" s="54"/>
+      <c r="I222" s="54"/>
+    </row>
+    <row r="223" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="8"/>
+      <c r="B223" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="C217" s="46"/>
-      <c r="D217" s="46"/>
-      <c r="E217" s="46"/>
-      <c r="F217" s="46"/>
-      <c r="G217" s="46"/>
-      <c r="H217" s="46"/>
-      <c r="I217" s="46"/>
-    </row>
-    <row r="218" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="8">
+      <c r="C223" s="54"/>
+      <c r="D223" s="54"/>
+      <c r="E223" s="54"/>
+      <c r="F223" s="54"/>
+      <c r="G223" s="54"/>
+      <c r="H223" s="54"/>
+      <c r="I223" s="54"/>
+    </row>
+    <row r="224" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A224" s="8">
         <v>6</v>
       </c>
-      <c r="B218" s="46" t="s">
+      <c r="B224" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C218" s="46"/>
-      <c r="D218" s="46"/>
-      <c r="E218" s="46"/>
-      <c r="F218" s="46"/>
-      <c r="G218" s="46"/>
-      <c r="H218" s="46"/>
-      <c r="I218" s="46"/>
-    </row>
-    <row r="219" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="8"/>
-      <c r="B219" s="46" t="s">
+      <c r="C224" s="54"/>
+      <c r="D224" s="54"/>
+      <c r="E224" s="54"/>
+      <c r="F224" s="54"/>
+      <c r="G224" s="54"/>
+      <c r="H224" s="54"/>
+      <c r="I224" s="54"/>
+    </row>
+    <row r="225" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="8"/>
+      <c r="B225" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C219" s="46"/>
-      <c r="D219" s="46"/>
-      <c r="E219" s="46"/>
-      <c r="F219" s="46"/>
-      <c r="G219" s="46"/>
-      <c r="H219" s="46"/>
-      <c r="I219" s="46"/>
-    </row>
-    <row r="220" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="8"/>
-      <c r="B220" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C220" s="46"/>
-      <c r="D220" s="46"/>
-      <c r="E220" s="46"/>
-      <c r="F220" s="46"/>
-      <c r="G220" s="46"/>
-      <c r="H220" s="46"/>
-      <c r="I220" s="46"/>
-    </row>
-    <row r="221" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="8">
-        <v>7</v>
-      </c>
-      <c r="B221" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="C221" s="46"/>
-      <c r="D221" s="46"/>
-      <c r="E221" s="46"/>
-      <c r="F221" s="46"/>
-      <c r="G221" s="46"/>
-      <c r="H221" s="46"/>
-      <c r="I221" s="46"/>
-    </row>
-    <row r="222" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="8">
-        <v>8</v>
-      </c>
-      <c r="B222" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="C222" s="46"/>
-      <c r="D222" s="46"/>
-      <c r="E222" s="46"/>
-      <c r="F222" s="46"/>
-      <c r="G222" s="46"/>
-      <c r="H222" s="46"/>
-      <c r="I222" s="46"/>
-    </row>
-    <row r="223" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="8"/>
-      <c r="B223" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C223" s="46"/>
-      <c r="D223" s="46"/>
-      <c r="E223" s="46"/>
-      <c r="F223" s="46"/>
-      <c r="G223" s="46"/>
-      <c r="H223" s="46"/>
-      <c r="I223" s="46"/>
-    </row>
-    <row r="224" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A224" s="8"/>
-      <c r="B224" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="C224" s="46"/>
-      <c r="D224" s="46"/>
-      <c r="E224" s="46"/>
-      <c r="F224" s="46"/>
-      <c r="G224" s="46"/>
-      <c r="H224" s="46"/>
-      <c r="I224" s="46"/>
-    </row>
-    <row r="225" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="8"/>
-      <c r="B225" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="C225" s="46"/>
-      <c r="D225" s="46"/>
-      <c r="E225" s="46"/>
-      <c r="F225" s="46"/>
-      <c r="G225" s="46"/>
-      <c r="H225" s="46"/>
-      <c r="I225" s="46"/>
+      <c r="C225" s="54"/>
+      <c r="D225" s="54"/>
+      <c r="E225" s="54"/>
+      <c r="F225" s="54"/>
+      <c r="G225" s="54"/>
+      <c r="H225" s="54"/>
+      <c r="I225" s="54"/>
     </row>
     <row r="226" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="8"/>
-      <c r="B226" s="46" t="s">
+      <c r="B226" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C226" s="54"/>
+      <c r="D226" s="54"/>
+      <c r="E226" s="54"/>
+      <c r="F226" s="54"/>
+      <c r="G226" s="54"/>
+      <c r="H226" s="54"/>
+      <c r="I226" s="54"/>
+    </row>
+    <row r="227" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="8">
+        <v>7</v>
+      </c>
+      <c r="B227" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="C227" s="54"/>
+      <c r="D227" s="54"/>
+      <c r="E227" s="54"/>
+      <c r="F227" s="54"/>
+      <c r="G227" s="54"/>
+      <c r="H227" s="54"/>
+      <c r="I227" s="54"/>
+    </row>
+    <row r="228" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="8">
+        <v>8</v>
+      </c>
+      <c r="B228" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="C228" s="54"/>
+      <c r="D228" s="54"/>
+      <c r="E228" s="54"/>
+      <c r="F228" s="54"/>
+      <c r="G228" s="54"/>
+      <c r="H228" s="54"/>
+      <c r="I228" s="54"/>
+    </row>
+    <row r="229" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="8"/>
+      <c r="B229" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="C229" s="54"/>
+      <c r="D229" s="54"/>
+      <c r="E229" s="54"/>
+      <c r="F229" s="54"/>
+      <c r="G229" s="54"/>
+      <c r="H229" s="54"/>
+      <c r="I229" s="54"/>
+    </row>
+    <row r="230" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="8"/>
+      <c r="B230" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C230" s="54"/>
+      <c r="D230" s="54"/>
+      <c r="E230" s="54"/>
+      <c r="F230" s="54"/>
+      <c r="G230" s="54"/>
+      <c r="H230" s="54"/>
+      <c r="I230" s="54"/>
+    </row>
+    <row r="231" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="8"/>
+      <c r="B231" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="C231" s="54"/>
+      <c r="D231" s="54"/>
+      <c r="E231" s="54"/>
+      <c r="F231" s="54"/>
+      <c r="G231" s="54"/>
+      <c r="H231" s="54"/>
+      <c r="I231" s="54"/>
+    </row>
+    <row r="232" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="8"/>
+      <c r="B232" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="C226" s="46"/>
-      <c r="D226" s="46"/>
-      <c r="E226" s="46"/>
-      <c r="F226" s="46"/>
-      <c r="G226" s="46"/>
-      <c r="H226" s="46"/>
-      <c r="I226" s="46"/>
-    </row>
-    <row r="227" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="8"/>
-      <c r="B227" s="46" t="s">
+      <c r="C232" s="54"/>
+      <c r="D232" s="54"/>
+      <c r="E232" s="54"/>
+      <c r="F232" s="54"/>
+      <c r="G232" s="54"/>
+      <c r="H232" s="54"/>
+      <c r="I232" s="54"/>
+    </row>
+    <row r="233" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="8"/>
+      <c r="B233" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="C227" s="46"/>
-      <c r="D227" s="46"/>
-      <c r="E227" s="46"/>
-      <c r="F227" s="46"/>
-      <c r="G227" s="46"/>
-      <c r="H227" s="46"/>
-      <c r="I227" s="46"/>
-    </row>
-    <row r="228" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="8"/>
-      <c r="B228" s="46" t="s">
+      <c r="C233" s="54"/>
+      <c r="D233" s="54"/>
+      <c r="E233" s="54"/>
+      <c r="F233" s="54"/>
+      <c r="G233" s="54"/>
+      <c r="H233" s="54"/>
+      <c r="I233" s="54"/>
+    </row>
+    <row r="234" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="8"/>
+      <c r="B234" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="C228" s="46"/>
-      <c r="D228" s="46"/>
-      <c r="E228" s="46"/>
-      <c r="F228" s="46"/>
-      <c r="G228" s="46"/>
-      <c r="H228" s="46"/>
-      <c r="I228" s="46"/>
-    </row>
-    <row r="229" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="8">
+      <c r="C234" s="54"/>
+      <c r="D234" s="54"/>
+      <c r="E234" s="54"/>
+      <c r="F234" s="54"/>
+      <c r="G234" s="54"/>
+      <c r="H234" s="54"/>
+      <c r="I234" s="54"/>
+    </row>
+    <row r="235" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="8">
         <v>9</v>
       </c>
-      <c r="B229" s="46" t="s">
+      <c r="B235" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="C229" s="46"/>
-      <c r="D229" s="46"/>
-      <c r="E229" s="46"/>
-      <c r="F229" s="46"/>
-      <c r="G229" s="46"/>
-      <c r="H229" s="46"/>
-      <c r="I229" s="46"/>
-    </row>
-    <row r="230" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="8">
+      <c r="C235" s="54"/>
+      <c r="D235" s="54"/>
+      <c r="E235" s="54"/>
+      <c r="F235" s="54"/>
+      <c r="G235" s="54"/>
+      <c r="H235" s="54"/>
+      <c r="I235" s="54"/>
+    </row>
+    <row r="236" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="8">
         <v>10</v>
       </c>
-      <c r="B230" s="46" t="s">
+      <c r="B236" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="C230" s="46"/>
-      <c r="D230" s="46"/>
-      <c r="E230" s="46"/>
-      <c r="F230" s="46"/>
-      <c r="G230" s="46"/>
-      <c r="H230" s="46"/>
-      <c r="I230" s="46"/>
-    </row>
-    <row r="231" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="8"/>
-      <c r="B231" s="46" t="s">
+      <c r="C236" s="54"/>
+      <c r="D236" s="54"/>
+      <c r="E236" s="54"/>
+      <c r="F236" s="54"/>
+      <c r="G236" s="54"/>
+      <c r="H236" s="54"/>
+      <c r="I236" s="54"/>
+    </row>
+    <row r="237" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="8"/>
+      <c r="B237" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="C231" s="46"/>
-      <c r="D231" s="46"/>
-      <c r="E231" s="46"/>
-      <c r="F231" s="46"/>
-      <c r="G231" s="46"/>
-      <c r="H231" s="46"/>
-      <c r="I231" s="46"/>
-    </row>
-    <row r="232" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="8"/>
-      <c r="B232" s="46" t="s">
+      <c r="C237" s="54"/>
+      <c r="D237" s="54"/>
+      <c r="E237" s="54"/>
+      <c r="F237" s="54"/>
+      <c r="G237" s="54"/>
+      <c r="H237" s="54"/>
+      <c r="I237" s="54"/>
+    </row>
+    <row r="238" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="8"/>
+      <c r="B238" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="C232" s="46"/>
-      <c r="D232" s="46"/>
-      <c r="E232" s="46"/>
-      <c r="F232" s="46"/>
-      <c r="G232" s="46"/>
-      <c r="H232" s="46"/>
-      <c r="I232" s="46"/>
-    </row>
-    <row r="233" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="8"/>
-      <c r="B233" s="46" t="s">
+      <c r="C238" s="54"/>
+      <c r="D238" s="54"/>
+      <c r="E238" s="54"/>
+      <c r="F238" s="54"/>
+      <c r="G238" s="54"/>
+      <c r="H238" s="54"/>
+      <c r="I238" s="54"/>
+    </row>
+    <row r="239" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="8"/>
+      <c r="B239" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="C233" s="46"/>
-      <c r="D233" s="46"/>
-      <c r="E233" s="46"/>
-      <c r="F233" s="46"/>
-      <c r="G233" s="46"/>
-      <c r="H233" s="46"/>
-      <c r="I233" s="46"/>
-    </row>
-    <row r="234" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="8"/>
-      <c r="B234" s="46" t="s">
+      <c r="C239" s="54"/>
+      <c r="D239" s="54"/>
+      <c r="E239" s="54"/>
+      <c r="F239" s="54"/>
+      <c r="G239" s="54"/>
+      <c r="H239" s="54"/>
+      <c r="I239" s="54"/>
+    </row>
+    <row r="240" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="8"/>
+      <c r="B240" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C234" s="46"/>
-      <c r="D234" s="46"/>
-      <c r="E234" s="46"/>
-      <c r="F234" s="46"/>
-      <c r="G234" s="46"/>
-      <c r="H234" s="46"/>
-      <c r="I234" s="46"/>
-    </row>
-    <row r="235" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="8">
+      <c r="C240" s="54"/>
+      <c r="D240" s="54"/>
+      <c r="E240" s="54"/>
+      <c r="F240" s="54"/>
+      <c r="G240" s="54"/>
+      <c r="H240" s="54"/>
+      <c r="I240" s="54"/>
+    </row>
+    <row r="241" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="8">
         <v>11</v>
       </c>
-      <c r="B235" s="46" t="s">
+      <c r="B241" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C235" s="46"/>
-      <c r="D235" s="46"/>
-      <c r="E235" s="46"/>
-      <c r="F235" s="46"/>
-      <c r="G235" s="46"/>
-      <c r="H235" s="46"/>
-      <c r="I235" s="46"/>
-    </row>
-    <row r="236" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="8"/>
-      <c r="B236" s="46" t="s">
+      <c r="C241" s="54"/>
+      <c r="D241" s="54"/>
+      <c r="E241" s="54"/>
+      <c r="F241" s="54"/>
+      <c r="G241" s="54"/>
+      <c r="H241" s="54"/>
+      <c r="I241" s="54"/>
+    </row>
+    <row r="242" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="8"/>
+      <c r="B242" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="C236" s="46"/>
-      <c r="D236" s="46"/>
-      <c r="E236" s="46"/>
-      <c r="F236" s="46"/>
-      <c r="G236" s="46"/>
-      <c r="H236" s="46"/>
-      <c r="I236" s="46"/>
-    </row>
-    <row r="237" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="8"/>
-      <c r="B237" s="46" t="s">
+      <c r="C242" s="54"/>
+      <c r="D242" s="54"/>
+      <c r="E242" s="54"/>
+      <c r="F242" s="54"/>
+      <c r="G242" s="54"/>
+      <c r="H242" s="54"/>
+      <c r="I242" s="54"/>
+    </row>
+    <row r="243" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="8"/>
+      <c r="B243" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="C237" s="46"/>
-      <c r="D237" s="46"/>
-      <c r="E237" s="46"/>
-      <c r="F237" s="46"/>
-      <c r="G237" s="46"/>
-      <c r="H237" s="46"/>
-      <c r="I237" s="46"/>
-    </row>
-    <row r="238" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="8">
+      <c r="C243" s="54"/>
+      <c r="D243" s="54"/>
+      <c r="E243" s="54"/>
+      <c r="F243" s="54"/>
+      <c r="G243" s="54"/>
+      <c r="H243" s="54"/>
+      <c r="I243" s="54"/>
+    </row>
+    <row r="244" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="8">
         <v>12</v>
       </c>
-      <c r="B238" s="46" t="s">
+      <c r="B244" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="C238" s="46"/>
-      <c r="D238" s="46"/>
-      <c r="E238" s="46"/>
-      <c r="F238" s="46"/>
-      <c r="G238" s="46"/>
-      <c r="H238" s="46"/>
-      <c r="I238" s="46"/>
-    </row>
-    <row r="239" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="8"/>
-      <c r="B239" s="46" t="s">
+      <c r="C244" s="54"/>
+      <c r="D244" s="54"/>
+      <c r="E244" s="54"/>
+      <c r="F244" s="54"/>
+      <c r="G244" s="54"/>
+      <c r="H244" s="54"/>
+      <c r="I244" s="54"/>
+    </row>
+    <row r="245" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="8"/>
+      <c r="B245" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="C239" s="46"/>
-      <c r="D239" s="46"/>
-      <c r="E239" s="46"/>
-      <c r="F239" s="46"/>
-      <c r="G239" s="46"/>
-      <c r="H239" s="46"/>
-      <c r="I239" s="46"/>
-    </row>
-    <row r="240" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="8"/>
-      <c r="B240" s="46" t="s">
+      <c r="C245" s="54"/>
+      <c r="D245" s="54"/>
+      <c r="E245" s="54"/>
+      <c r="F245" s="54"/>
+      <c r="G245" s="54"/>
+      <c r="H245" s="54"/>
+      <c r="I245" s="54"/>
+    </row>
+    <row r="246" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="8"/>
+      <c r="B246" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="C240" s="46"/>
-      <c r="D240" s="46"/>
-      <c r="E240" s="46"/>
-      <c r="F240" s="46"/>
-      <c r="G240" s="46"/>
-      <c r="H240" s="46"/>
-      <c r="I240" s="46"/>
-    </row>
-    <row r="241" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="8"/>
-      <c r="B241" s="46" t="s">
+      <c r="C246" s="54"/>
+      <c r="D246" s="54"/>
+      <c r="E246" s="54"/>
+      <c r="F246" s="54"/>
+      <c r="G246" s="54"/>
+      <c r="H246" s="54"/>
+      <c r="I246" s="54"/>
+    </row>
+    <row r="247" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="8"/>
+      <c r="B247" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="C241" s="46"/>
-      <c r="D241" s="46"/>
-      <c r="E241" s="46"/>
-      <c r="F241" s="46"/>
-      <c r="G241" s="46"/>
-      <c r="H241" s="46"/>
-      <c r="I241" s="46"/>
-    </row>
-    <row r="242" spans="1:9" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="8"/>
-      <c r="B242" s="46" t="s">
+      <c r="C247" s="54"/>
+      <c r="D247" s="54"/>
+      <c r="E247" s="54"/>
+      <c r="F247" s="54"/>
+      <c r="G247" s="54"/>
+      <c r="H247" s="54"/>
+      <c r="I247" s="54"/>
+    </row>
+    <row r="248" spans="1:9" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="8"/>
+      <c r="B248" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C242" s="46"/>
-      <c r="D242" s="46"/>
-      <c r="E242" s="46"/>
-      <c r="F242" s="46"/>
-      <c r="G242" s="46"/>
-      <c r="H242" s="46"/>
-      <c r="I242" s="46"/>
-    </row>
-    <row r="243" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="8">
+      <c r="C248" s="54"/>
+      <c r="D248" s="54"/>
+      <c r="E248" s="54"/>
+      <c r="F248" s="54"/>
+      <c r="G248" s="54"/>
+      <c r="H248" s="54"/>
+      <c r="I248" s="54"/>
+    </row>
+    <row r="249" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="8">
         <v>13</v>
       </c>
-      <c r="B243" s="46" t="s">
+      <c r="B249" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C243" s="46"/>
-      <c r="D243" s="46"/>
-      <c r="E243" s="46"/>
-      <c r="F243" s="46"/>
-      <c r="G243" s="46"/>
-      <c r="H243" s="46"/>
-      <c r="I243" s="46"/>
-    </row>
-    <row r="244" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="8"/>
-      <c r="B244" s="46" t="s">
+      <c r="C249" s="54"/>
+      <c r="D249" s="54"/>
+      <c r="E249" s="54"/>
+      <c r="F249" s="54"/>
+      <c r="G249" s="54"/>
+      <c r="H249" s="54"/>
+      <c r="I249" s="54"/>
+    </row>
+    <row r="250" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="8"/>
+      <c r="B250" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="C244" s="46"/>
-      <c r="D244" s="46"/>
-      <c r="E244" s="46"/>
-      <c r="F244" s="46"/>
-      <c r="G244" s="46"/>
-      <c r="H244" s="46"/>
-      <c r="I244" s="46"/>
-    </row>
-    <row r="245" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="8"/>
-      <c r="B245" s="46" t="s">
+      <c r="C250" s="54"/>
+      <c r="D250" s="54"/>
+      <c r="E250" s="54"/>
+      <c r="F250" s="54"/>
+      <c r="G250" s="54"/>
+      <c r="H250" s="54"/>
+      <c r="I250" s="54"/>
+    </row>
+    <row r="251" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="8"/>
+      <c r="B251" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="C245" s="46"/>
-      <c r="D245" s="46"/>
-      <c r="E245" s="46"/>
-      <c r="F245" s="46"/>
-      <c r="G245" s="46"/>
-      <c r="H245" s="46"/>
-      <c r="I245" s="46"/>
-    </row>
-    <row r="246" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="8">
+      <c r="C251" s="54"/>
+      <c r="D251" s="54"/>
+      <c r="E251" s="54"/>
+      <c r="F251" s="54"/>
+      <c r="G251" s="54"/>
+      <c r="H251" s="54"/>
+      <c r="I251" s="54"/>
+    </row>
+    <row r="252" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="8">
         <v>14</v>
       </c>
-      <c r="B246" s="46" t="s">
+      <c r="B252" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="C246" s="46"/>
-      <c r="D246" s="46"/>
-      <c r="E246" s="46"/>
-      <c r="F246" s="46"/>
-      <c r="G246" s="46"/>
-      <c r="H246" s="46"/>
-      <c r="I246" s="46"/>
-    </row>
-    <row r="247" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="8"/>
-      <c r="B247" s="46" t="s">
+      <c r="C252" s="54"/>
+      <c r="D252" s="54"/>
+      <c r="E252" s="54"/>
+      <c r="F252" s="54"/>
+      <c r="G252" s="54"/>
+      <c r="H252" s="54"/>
+      <c r="I252" s="54"/>
+    </row>
+    <row r="253" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="8"/>
+      <c r="B253" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="C247" s="46"/>
-      <c r="D247" s="46"/>
-      <c r="E247" s="46"/>
-      <c r="F247" s="46"/>
-      <c r="G247" s="46"/>
-      <c r="H247" s="46"/>
-      <c r="I247" s="46"/>
-    </row>
-    <row r="248" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="8"/>
-      <c r="B248" s="46" t="s">
+      <c r="C253" s="54"/>
+      <c r="D253" s="54"/>
+      <c r="E253" s="54"/>
+      <c r="F253" s="54"/>
+      <c r="G253" s="54"/>
+      <c r="H253" s="54"/>
+      <c r="I253" s="54"/>
+    </row>
+    <row r="254" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="8"/>
+      <c r="B254" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="C248" s="46"/>
-      <c r="D248" s="46"/>
-      <c r="E248" s="46"/>
-      <c r="F248" s="46"/>
-      <c r="G248" s="46"/>
-      <c r="H248" s="46"/>
-      <c r="I248" s="46"/>
-    </row>
-    <row r="249" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="8"/>
-      <c r="B249" s="46" t="s">
+      <c r="C254" s="54"/>
+      <c r="D254" s="54"/>
+      <c r="E254" s="54"/>
+      <c r="F254" s="54"/>
+      <c r="G254" s="54"/>
+      <c r="H254" s="54"/>
+      <c r="I254" s="54"/>
+    </row>
+    <row r="255" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="8"/>
+      <c r="B255" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="C249" s="46"/>
-      <c r="D249" s="46"/>
-      <c r="E249" s="46"/>
-      <c r="F249" s="46"/>
-      <c r="G249" s="46"/>
-      <c r="H249" s="46"/>
-      <c r="I249" s="46"/>
-    </row>
-    <row r="250" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="8"/>
-      <c r="B250" s="46" t="s">
+      <c r="C255" s="54"/>
+      <c r="D255" s="54"/>
+      <c r="E255" s="54"/>
+      <c r="F255" s="54"/>
+      <c r="G255" s="54"/>
+      <c r="H255" s="54"/>
+      <c r="I255" s="54"/>
+    </row>
+    <row r="256" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="8"/>
+      <c r="B256" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="C250" s="46"/>
-      <c r="D250" s="46"/>
-      <c r="E250" s="46"/>
-      <c r="F250" s="46"/>
-      <c r="G250" s="46"/>
-      <c r="H250" s="46"/>
-      <c r="I250" s="46"/>
-    </row>
-    <row r="251" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="8">
+      <c r="C256" s="54"/>
+      <c r="D256" s="54"/>
+      <c r="E256" s="54"/>
+      <c r="F256" s="54"/>
+      <c r="G256" s="54"/>
+      <c r="H256" s="54"/>
+      <c r="I256" s="54"/>
+    </row>
+    <row r="257" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="8">
         <v>15</v>
       </c>
-      <c r="B251" s="46" t="s">
+      <c r="B257" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="C251" s="46"/>
-      <c r="D251" s="46"/>
-      <c r="E251" s="46"/>
-      <c r="F251" s="46"/>
-      <c r="G251" s="46"/>
-      <c r="H251" s="46"/>
-      <c r="I251" s="46"/>
-    </row>
-    <row r="252" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="8">
+      <c r="C257" s="54"/>
+      <c r="D257" s="54"/>
+      <c r="E257" s="54"/>
+      <c r="F257" s="54"/>
+      <c r="G257" s="54"/>
+      <c r="H257" s="54"/>
+      <c r="I257" s="54"/>
+    </row>
+    <row r="258" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="8">
         <v>16</v>
       </c>
-      <c r="B252" s="46" t="s">
+      <c r="B258" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="C252" s="46"/>
-      <c r="D252" s="46"/>
-      <c r="E252" s="46"/>
-      <c r="F252" s="46"/>
-      <c r="G252" s="46"/>
-      <c r="H252" s="46"/>
-      <c r="I252" s="46"/>
-    </row>
-    <row r="253" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A253" s="8">
+      <c r="C258" s="54"/>
+      <c r="D258" s="54"/>
+      <c r="E258" s="54"/>
+      <c r="F258" s="54"/>
+      <c r="G258" s="54"/>
+      <c r="H258" s="54"/>
+      <c r="I258" s="54"/>
+    </row>
+    <row r="259" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="8">
         <v>17</v>
       </c>
-      <c r="B253" s="46" t="s">
+      <c r="B259" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="C253" s="46"/>
-      <c r="D253" s="46"/>
-      <c r="E253" s="46"/>
-      <c r="F253" s="46"/>
-      <c r="G253" s="46"/>
-      <c r="H253" s="46"/>
-      <c r="I253" s="46"/>
-    </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A254" s="27"/>
-    </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A255" s="27"/>
-    </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A256" s="27"/>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" s="27"/>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="27"/>
+      <c r="C259" s="54"/>
+      <c r="D259" s="54"/>
+      <c r="E259" s="54"/>
+      <c r="F259" s="54"/>
+      <c r="G259" s="54"/>
+      <c r="H259" s="54"/>
+      <c r="I259" s="54"/>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A260" s="27"/>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A261" s="27"/>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A262" s="27"/>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A263" s="27"/>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A264" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="B141:I141"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B132:I133"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B126:I129"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="B29:I29"/>
-    <mergeCell ref="B32:I32"/>
-    <mergeCell ref="B33:I33"/>
-    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="B259:I259"/>
+    <mergeCell ref="C185:E185"/>
+    <mergeCell ref="B172:I175"/>
+    <mergeCell ref="B160:I160"/>
+    <mergeCell ref="B179:I180"/>
+    <mergeCell ref="F166:G166"/>
+    <mergeCell ref="F167:G167"/>
+    <mergeCell ref="F168:G168"/>
+    <mergeCell ref="D166:E166"/>
+    <mergeCell ref="D167:E167"/>
+    <mergeCell ref="D168:E168"/>
+    <mergeCell ref="B165:I165"/>
+    <mergeCell ref="B181:E181"/>
+    <mergeCell ref="B182:E182"/>
+    <mergeCell ref="B183:E183"/>
+    <mergeCell ref="B184:E184"/>
+    <mergeCell ref="B216:I216"/>
+    <mergeCell ref="B217:I217"/>
+    <mergeCell ref="B218:I218"/>
+    <mergeCell ref="B219:I219"/>
+    <mergeCell ref="B220:I220"/>
+    <mergeCell ref="F214:G214"/>
+    <mergeCell ref="B188:I190"/>
+    <mergeCell ref="B234:I234"/>
+    <mergeCell ref="B221:I221"/>
+    <mergeCell ref="B222:I222"/>
+    <mergeCell ref="B223:I223"/>
+    <mergeCell ref="B224:I224"/>
+    <mergeCell ref="B230:I230"/>
+    <mergeCell ref="B225:I225"/>
+    <mergeCell ref="B226:I226"/>
+    <mergeCell ref="B227:I227"/>
+    <mergeCell ref="B228:I228"/>
+    <mergeCell ref="B229:I229"/>
+    <mergeCell ref="B231:I231"/>
+    <mergeCell ref="B232:I232"/>
+    <mergeCell ref="B233:I233"/>
+    <mergeCell ref="B246:I246"/>
+    <mergeCell ref="B235:I235"/>
+    <mergeCell ref="B236:I236"/>
+    <mergeCell ref="B237:I237"/>
+    <mergeCell ref="B238:I238"/>
+    <mergeCell ref="B239:I239"/>
+    <mergeCell ref="B240:I240"/>
+    <mergeCell ref="B241:I241"/>
+    <mergeCell ref="B242:I242"/>
+    <mergeCell ref="B243:I243"/>
+    <mergeCell ref="B244:I244"/>
+    <mergeCell ref="B245:I245"/>
+    <mergeCell ref="B258:I258"/>
+    <mergeCell ref="B247:I247"/>
+    <mergeCell ref="B248:I248"/>
+    <mergeCell ref="B249:I249"/>
+    <mergeCell ref="B250:I250"/>
+    <mergeCell ref="B251:I251"/>
+    <mergeCell ref="B252:I252"/>
+    <mergeCell ref="B253:I253"/>
+    <mergeCell ref="B254:I254"/>
+    <mergeCell ref="B255:I255"/>
+    <mergeCell ref="B256:I256"/>
+    <mergeCell ref="B257:I257"/>
     <mergeCell ref="Q9:X9"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="K2:L2"/>
@@ -4308,67 +4408,21 @@
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="A8:I9"/>
     <mergeCell ref="A6:I6"/>
-    <mergeCell ref="B252:I252"/>
-    <mergeCell ref="B241:I241"/>
-    <mergeCell ref="B242:I242"/>
-    <mergeCell ref="B243:I243"/>
-    <mergeCell ref="B244:I244"/>
-    <mergeCell ref="B245:I245"/>
-    <mergeCell ref="B246:I246"/>
-    <mergeCell ref="B247:I247"/>
-    <mergeCell ref="B248:I248"/>
-    <mergeCell ref="B249:I249"/>
-    <mergeCell ref="B250:I250"/>
-    <mergeCell ref="B251:I251"/>
-    <mergeCell ref="B240:I240"/>
-    <mergeCell ref="B229:I229"/>
-    <mergeCell ref="B230:I230"/>
-    <mergeCell ref="B231:I231"/>
-    <mergeCell ref="B232:I232"/>
-    <mergeCell ref="B233:I233"/>
-    <mergeCell ref="B234:I234"/>
-    <mergeCell ref="B235:I235"/>
-    <mergeCell ref="B236:I236"/>
-    <mergeCell ref="B237:I237"/>
-    <mergeCell ref="B238:I238"/>
-    <mergeCell ref="B239:I239"/>
-    <mergeCell ref="F208:G208"/>
-    <mergeCell ref="B182:I184"/>
-    <mergeCell ref="B228:I228"/>
-    <mergeCell ref="B215:I215"/>
-    <mergeCell ref="B216:I216"/>
-    <mergeCell ref="B217:I217"/>
-    <mergeCell ref="B218:I218"/>
-    <mergeCell ref="B224:I224"/>
-    <mergeCell ref="B219:I219"/>
-    <mergeCell ref="B220:I220"/>
-    <mergeCell ref="B221:I221"/>
-    <mergeCell ref="B222:I222"/>
-    <mergeCell ref="B223:I223"/>
-    <mergeCell ref="B225:I225"/>
-    <mergeCell ref="B226:I226"/>
-    <mergeCell ref="B227:I227"/>
-    <mergeCell ref="B210:I210"/>
-    <mergeCell ref="B211:I211"/>
-    <mergeCell ref="B212:I212"/>
-    <mergeCell ref="B213:I213"/>
-    <mergeCell ref="B214:I214"/>
-    <mergeCell ref="B253:I253"/>
-    <mergeCell ref="C179:E179"/>
-    <mergeCell ref="B166:I169"/>
-    <mergeCell ref="B154:I154"/>
-    <mergeCell ref="B173:I174"/>
-    <mergeCell ref="F160:G160"/>
-    <mergeCell ref="F161:G161"/>
-    <mergeCell ref="F162:G162"/>
-    <mergeCell ref="D160:E160"/>
-    <mergeCell ref="D161:E161"/>
-    <mergeCell ref="D162:E162"/>
-    <mergeCell ref="B159:I159"/>
-    <mergeCell ref="B175:E175"/>
-    <mergeCell ref="B176:E176"/>
-    <mergeCell ref="B177:E177"/>
-    <mergeCell ref="B178:E178"/>
+    <mergeCell ref="B147:I147"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B138:I139"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B132:I135"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="B34:I34"/>
   </mergeCells>
   <conditionalFormatting sqref="B17">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
@@ -4389,8 +4443,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A35 A25" xr:uid="{2610830F-8508-4F02-A4A6-401E578A5A49}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="UNLISTED ITEM" error="Please input customised items manually" sqref="B134:B138" xr:uid="{92AF6CB7-4A80-4E2F-8377-0310E8DEBE08}"/>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="UNLISTED ITEM" error="Please input customised items manually" sqref="C123:I123 A123 B69:B75 B53:B67 J77:XFD123 B77:B123" xr:uid="{227805A3-D203-44AE-9483-BFAA5260215C}">
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="UNLISTED ITEM" error="Please input customised items manually" sqref="B140:B144" xr:uid="{92AF6CB7-4A80-4E2F-8377-0310E8DEBE08}"/>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="UNLISTED ITEM" error="Please input customised items manually" sqref="C129:I129 A129 B69:B75 B53:B67 J77:XFD129 B77:B129" xr:uid="{227805A3-D203-44AE-9483-BFAA5260215C}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -4412,10 +4466,10 @@
   <rowBreaks count="6" manualBreakCount="6">
     <brk id="43" max="8" man="1"/>
     <brk id="83" max="8" man="1"/>
-    <brk id="123" max="8" man="1"/>
-    <brk id="164" max="8" man="1"/>
-    <brk id="208" max="8" man="1"/>
-    <brk id="231" max="8" man="1"/>
+    <brk id="129" max="8" man="1"/>
+    <brk id="170" max="8" man="1"/>
+    <brk id="214" max="8" man="1"/>
+    <brk id="237" max="8" man="1"/>
   </rowBreaks>
   <drawing r:id="rId4"/>
   <legacyDrawingHF r:id="rId5"/>

</xml_diff>